<commit_message>
Updated R script for SVA and batch effect correction
</commit_message>
<xml_diff>
--- a/Proteomics/Terminal/data/metadata/meta_proteomics.xlsx
+++ b/Proteomics/Terminal/data/metadata/meta_proteomics.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nks882\OneDrive - University of Copenhagen\Documents\GitHub\Horse_AF_project\mass_spec\placebo_vs_sham\data\metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumni-my.sharepoint.com/personal/nks882_ku_dk/Documents/Documents/GitHub/Horse_Metformin_Project/Proteomics/Terminal/data/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19030" windowHeight="6540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17270"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="100">
   <si>
     <t>Region</t>
   </si>
@@ -306,6 +309,24 @@
   </si>
   <si>
     <t>Horse</t>
+  </si>
+  <si>
+    <t>Age</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Batch</t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Gelding</t>
+  </si>
+  <si>
+    <t>Mare</t>
   </si>
 </sst>
 </file>
@@ -650,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F73"/>
+  <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -661,9 +682,12 @@
     <col min="1" max="1" width="59.1796875" customWidth="1"/>
     <col min="3" max="5" width="16.54296875" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" customWidth="1"/>
+    <col min="7" max="7" width="14.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.1796875" customWidth="1"/>
+    <col min="9" max="9" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>91</v>
       </c>
@@ -682,8 +706,20 @@
       <c r="F1" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -702,8 +738,20 @@
       <c r="F2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
@@ -722,8 +770,20 @@
       <c r="F3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>98</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -742,8 +802,20 @@
       <c r="F4" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>98</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -762,8 +834,20 @@
       <c r="F5" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>99</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -782,8 +866,20 @@
       <c r="F6" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6" t="s">
+        <v>99</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -802,8 +898,20 @@
       <c r="F7" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>99</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
@@ -822,8 +930,20 @@
       <c r="F8" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>5</v>
+      </c>
+      <c r="H8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -842,8 +962,20 @@
       <c r="F9" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>99</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
@@ -862,8 +994,20 @@
       <c r="F10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>5</v>
+      </c>
+      <c r="H10" t="s">
+        <v>99</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -882,8 +1026,20 @@
       <c r="F11" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11" t="s">
+        <v>99</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
@@ -902,8 +1058,20 @@
       <c r="F12" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -922,8 +1090,20 @@
       <c r="F13" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>99</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -942,8 +1122,20 @@
       <c r="F14" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
+        <v>98</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
@@ -962,8 +1154,20 @@
       <c r="F15" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
@@ -982,8 +1186,20 @@
       <c r="F16" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
@@ -1002,8 +1218,20 @@
       <c r="F17" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>99</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
@@ -1022,8 +1250,20 @@
       <c r="F18" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
@@ -1042,8 +1282,20 @@
       <c r="F19" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>99</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
@@ -1062,8 +1314,20 @@
       <c r="F20" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>5</v>
+      </c>
+      <c r="H20" t="s">
+        <v>99</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
@@ -1082,8 +1346,20 @@
       <c r="F21" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>5</v>
+      </c>
+      <c r="H21" t="s">
+        <v>99</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
@@ -1102,8 +1378,20 @@
       <c r="F22" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>99</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
@@ -1122,8 +1410,20 @@
       <c r="F23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>98</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
@@ -1142,8 +1442,20 @@
       <c r="F24" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="H24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
@@ -1162,8 +1474,20 @@
       <c r="F25" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>5</v>
+      </c>
+      <c r="H25" t="s">
+        <v>98</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
@@ -1182,8 +1506,20 @@
       <c r="F26" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>98</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
@@ -1202,8 +1538,20 @@
       <c r="F27" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>98</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
@@ -1222,8 +1570,20 @@
       <c r="F28" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
+        <v>98</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="2" t="s">
         <v>33</v>
       </c>
@@ -1242,8 +1602,20 @@
       <c r="F29" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>10</v>
+      </c>
+      <c r="H29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
@@ -1262,8 +1634,20 @@
       <c r="F30" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30" t="s">
+        <v>98</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
@@ -1282,8 +1666,20 @@
       <c r="F31" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31" t="s">
+        <v>98</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
@@ -1302,8 +1698,20 @@
       <c r="F32" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>9</v>
+      </c>
+      <c r="H32" t="s">
+        <v>99</v>
+      </c>
+      <c r="I32">
+        <v>3</v>
+      </c>
+      <c r="J32">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
@@ -1322,8 +1730,20 @@
       <c r="F33" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>9</v>
+      </c>
+      <c r="H33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33">
+        <v>3</v>
+      </c>
+      <c r="J33">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
@@ -1342,8 +1762,20 @@
       <c r="F34" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>9</v>
+      </c>
+      <c r="H34" t="s">
+        <v>99</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
@@ -1362,8 +1794,20 @@
       <c r="F35" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>8</v>
+      </c>
+      <c r="H35" t="s">
+        <v>99</v>
+      </c>
+      <c r="I35">
+        <v>3</v>
+      </c>
+      <c r="J35">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
@@ -1382,8 +1826,20 @@
       <c r="F36" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>8</v>
+      </c>
+      <c r="H36" t="s">
+        <v>99</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="J36">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
@@ -1402,8 +1858,20 @@
       <c r="F37" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>8</v>
+      </c>
+      <c r="H37" t="s">
+        <v>99</v>
+      </c>
+      <c r="I37">
+        <v>3</v>
+      </c>
+      <c r="J37">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
@@ -1422,8 +1890,20 @@
       <c r="F38" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>7</v>
+      </c>
+      <c r="H38" t="s">
+        <v>99</v>
+      </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
@@ -1442,8 +1922,20 @@
       <c r="F39" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>7</v>
+      </c>
+      <c r="H39" t="s">
+        <v>99</v>
+      </c>
+      <c r="I39">
+        <v>3</v>
+      </c>
+      <c r="J39">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
@@ -1462,8 +1954,20 @@
       <c r="F40" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>7</v>
+      </c>
+      <c r="H40" t="s">
+        <v>99</v>
+      </c>
+      <c r="I40">
+        <v>3</v>
+      </c>
+      <c r="J40">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
@@ -1482,8 +1986,20 @@
       <c r="F41" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>6</v>
+      </c>
+      <c r="H41" t="s">
+        <v>98</v>
+      </c>
+      <c r="I41">
+        <v>3</v>
+      </c>
+      <c r="J41">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
@@ -1502,8 +2018,20 @@
       <c r="F42" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>6</v>
+      </c>
+      <c r="H42" t="s">
+        <v>98</v>
+      </c>
+      <c r="I42">
+        <v>3</v>
+      </c>
+      <c r="J42">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
@@ -1522,8 +2050,20 @@
       <c r="F43" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43" t="s">
+        <v>98</v>
+      </c>
+      <c r="I43">
+        <v>3</v>
+      </c>
+      <c r="J43">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
@@ -1542,8 +2082,20 @@
       <c r="F44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>7</v>
+      </c>
+      <c r="H44" t="s">
+        <v>99</v>
+      </c>
+      <c r="I44">
+        <v>3</v>
+      </c>
+      <c r="J44">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
@@ -1562,8 +2114,20 @@
       <c r="F45" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>7</v>
+      </c>
+      <c r="H45" t="s">
+        <v>99</v>
+      </c>
+      <c r="I45">
+        <v>3</v>
+      </c>
+      <c r="J45">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
@@ -1582,8 +2146,20 @@
       <c r="F46" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>7</v>
+      </c>
+      <c r="H46" t="s">
+        <v>99</v>
+      </c>
+      <c r="I46">
+        <v>3</v>
+      </c>
+      <c r="J46">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
@@ -1602,8 +2178,20 @@
       <c r="F47" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>8</v>
+      </c>
+      <c r="H47" t="s">
+        <v>98</v>
+      </c>
+      <c r="I47">
+        <v>3</v>
+      </c>
+      <c r="J47">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
@@ -1622,8 +2210,20 @@
       <c r="F48" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>8</v>
+      </c>
+      <c r="H48" t="s">
+        <v>98</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
@@ -1642,8 +2242,20 @@
       <c r="F49" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>8</v>
+      </c>
+      <c r="H49" t="s">
+        <v>98</v>
+      </c>
+      <c r="I49">
+        <v>3</v>
+      </c>
+      <c r="J49">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -1662,8 +2274,20 @@
       <c r="F50" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>6</v>
+      </c>
+      <c r="H50" t="s">
+        <v>99</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
@@ -1682,8 +2306,20 @@
       <c r="F51" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>6</v>
+      </c>
+      <c r="H51" t="s">
+        <v>99</v>
+      </c>
+      <c r="I51">
+        <v>3</v>
+      </c>
+      <c r="J51">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
@@ -1702,8 +2338,20 @@
       <c r="F52" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>6</v>
+      </c>
+      <c r="H52" t="s">
+        <v>99</v>
+      </c>
+      <c r="I52">
+        <v>3</v>
+      </c>
+      <c r="J52">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>57</v>
       </c>
@@ -1722,8 +2370,20 @@
       <c r="F53" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>6</v>
+      </c>
+      <c r="H53" t="s">
+        <v>99</v>
+      </c>
+      <c r="I53">
+        <v>4</v>
+      </c>
+      <c r="J53">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -1742,8 +2402,20 @@
       <c r="F54" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <v>6</v>
+      </c>
+      <c r="H54" t="s">
+        <v>99</v>
+      </c>
+      <c r="I54">
+        <v>4</v>
+      </c>
+      <c r="J54">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="2" t="s">
         <v>59</v>
       </c>
@@ -1762,8 +2434,20 @@
       <c r="F55" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <v>6</v>
+      </c>
+      <c r="H55" t="s">
+        <v>99</v>
+      </c>
+      <c r="I55">
+        <v>4</v>
+      </c>
+      <c r="J55">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="2" t="s">
         <v>60</v>
       </c>
@@ -1782,8 +2466,20 @@
       <c r="F56" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <v>5</v>
+      </c>
+      <c r="H56" t="s">
+        <v>99</v>
+      </c>
+      <c r="I56">
+        <v>4</v>
+      </c>
+      <c r="J56">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A57" s="2" t="s">
         <v>61</v>
       </c>
@@ -1802,8 +2498,20 @@
       <c r="F57" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>5</v>
+      </c>
+      <c r="H57" t="s">
+        <v>99</v>
+      </c>
+      <c r="I57">
+        <v>4</v>
+      </c>
+      <c r="J57">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="2" t="s">
         <v>62</v>
       </c>
@@ -1822,8 +2530,20 @@
       <c r="F58" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>5</v>
+      </c>
+      <c r="H58" t="s">
+        <v>99</v>
+      </c>
+      <c r="I58">
+        <v>4</v>
+      </c>
+      <c r="J58">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="2" t="s">
         <v>63</v>
       </c>
@@ -1842,8 +2562,20 @@
       <c r="F59" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <v>6</v>
+      </c>
+      <c r="H59" t="s">
+        <v>99</v>
+      </c>
+      <c r="I59">
+        <v>4</v>
+      </c>
+      <c r="J59">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="2" t="s">
         <v>64</v>
       </c>
@@ -1862,8 +2594,20 @@
       <c r="F60" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <v>6</v>
+      </c>
+      <c r="H60" t="s">
+        <v>99</v>
+      </c>
+      <c r="I60">
+        <v>4</v>
+      </c>
+      <c r="J60">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="2" t="s">
         <v>65</v>
       </c>
@@ -1882,8 +2626,20 @@
       <c r="F61" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <v>6</v>
+      </c>
+      <c r="H61" t="s">
+        <v>99</v>
+      </c>
+      <c r="I61">
+        <v>4</v>
+      </c>
+      <c r="J61">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="2" t="s">
         <v>66</v>
       </c>
@@ -1902,8 +2658,20 @@
       <c r="F62" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <v>5</v>
+      </c>
+      <c r="H62" t="s">
+        <v>99</v>
+      </c>
+      <c r="I62">
+        <v>4</v>
+      </c>
+      <c r="J62">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="2" t="s">
         <v>67</v>
       </c>
@@ -1922,8 +2690,20 @@
       <c r="F63" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <v>5</v>
+      </c>
+      <c r="H63" t="s">
+        <v>99</v>
+      </c>
+      <c r="I63">
+        <v>4</v>
+      </c>
+      <c r="J63">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A64" s="2" t="s">
         <v>68</v>
       </c>
@@ -1942,8 +2722,20 @@
       <c r="F64" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <v>5</v>
+      </c>
+      <c r="H64" t="s">
+        <v>99</v>
+      </c>
+      <c r="I64">
+        <v>4</v>
+      </c>
+      <c r="J64">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="2" t="s">
         <v>69</v>
       </c>
@@ -1962,8 +2754,20 @@
       <c r="F65" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <v>8</v>
+      </c>
+      <c r="H65" t="s">
+        <v>99</v>
+      </c>
+      <c r="I65">
+        <v>4</v>
+      </c>
+      <c r="J65">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="2" t="s">
         <v>70</v>
       </c>
@@ -1982,8 +2786,20 @@
       <c r="F66" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <v>8</v>
+      </c>
+      <c r="H66" t="s">
+        <v>99</v>
+      </c>
+      <c r="I66">
+        <v>4</v>
+      </c>
+      <c r="J66">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="2" t="s">
         <v>71</v>
       </c>
@@ -2002,8 +2818,20 @@
       <c r="F67" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <v>8</v>
+      </c>
+      <c r="H67" t="s">
+        <v>99</v>
+      </c>
+      <c r="I67">
+        <v>4</v>
+      </c>
+      <c r="J67">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="2" t="s">
         <v>72</v>
       </c>
@@ -2022,8 +2850,20 @@
       <c r="F68" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68">
+        <v>8</v>
+      </c>
+      <c r="H68" t="s">
+        <v>99</v>
+      </c>
+      <c r="I68">
+        <v>4</v>
+      </c>
+      <c r="J68">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="2" t="s">
         <v>73</v>
       </c>
@@ -2042,8 +2882,20 @@
       <c r="F69" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69">
+        <v>8</v>
+      </c>
+      <c r="H69" t="s">
+        <v>99</v>
+      </c>
+      <c r="I69">
+        <v>4</v>
+      </c>
+      <c r="J69">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="2" t="s">
         <v>74</v>
       </c>
@@ -2062,8 +2914,20 @@
       <c r="F70" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>8</v>
+      </c>
+      <c r="H70" t="s">
+        <v>99</v>
+      </c>
+      <c r="I70">
+        <v>4</v>
+      </c>
+      <c r="J70">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="2" t="s">
         <v>75</v>
       </c>
@@ -2082,8 +2946,20 @@
       <c r="F71" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <v>4</v>
+      </c>
+      <c r="H71" t="s">
+        <v>99</v>
+      </c>
+      <c r="I71">
+        <v>4</v>
+      </c>
+      <c r="J71">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>76</v>
       </c>
@@ -2102,8 +2978,20 @@
       <c r="F72" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="H72" t="s">
+        <v>99</v>
+      </c>
+      <c r="I72">
+        <v>4</v>
+      </c>
+      <c r="J72">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
@@ -2122,28 +3010,41 @@
       <c r="F73" t="s">
         <v>90</v>
       </c>
+      <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73" t="s">
+        <v>99</v>
+      </c>
+      <c r="I73">
+        <v>4</v>
+      </c>
+      <c r="J73">
+        <v>445</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="4b43a846-4517-4017-9f6b-0674e58d3a61" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="4b43a846-4517-4017-9f6b-0674e58d3a61" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2374,26 +3275,26 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08126BC-C70B-4151-95C7-19633FD0C554}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{672617F7-CD14-4BF1-A783-7C626279C46D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="4b43a846-4517-4017-9f6b-0674e58d3a61"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="50d64243-e380-43e3-8d8f-39b0e9df45ae"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{672617F7-CD14-4BF1-A783-7C626279C46D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A08126BC-C70B-4151-95C7-19633FD0C554}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="50d64243-e380-43e3-8d8f-39b0e9df45ae"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4b43a846-4517-4017-9f6b-0674e58d3a61"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>